<commit_message>
2a Reunião - Decisões
A equipe discutiu sobre as sugestõesindividuais de cada integrante para tomarmos as decisões
</commit_message>
<xml_diff>
--- a/[The IFPR Brat Pack] Planilha de Decisões Arquiteturais.xlsx
+++ b/[The IFPR Brat Pack] Planilha de Decisões Arquiteturais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudos\ES 3° ANO\Arquitetura e Padrões de Software\arqps-automacao-residencial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C0F784-1238-4176-B2EB-1E499C51C3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EA6A6D-10BD-494C-BD6E-CC8D06F67470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="1785" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preocupações" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="193">
   <si>
     <t>Preocupações, Requisitos Funcionais e Requisitos Não-Funcionais Importantes para a Arquitetura</t>
   </si>
@@ -313,9 +313,6 @@
     <t>(--)</t>
   </si>
   <si>
-    <t>Em um hard-drive no local, para prevenir os casos de falta de energia e internet, e na nuvem utilizando o AWS Cloud Storage</t>
-  </si>
-  <si>
     <t>A escolha do AWS Cloud Storage deve-se ao fato desse serviço estar disponível em vários países</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>Essa decisão foi tomada pensando em garantir Cibersegurança e ganhar tempo no desenvolvimento, não precisando desenvolver nossas próprias ferramentas, utilizando ferramentas prontas e confiáveis.</t>
   </si>
   <si>
-    <t xml:space="preserve">RNF - Deverá ser implementado um sistema mobile para controle dos módulos, visando facilitar o uso dos usuários e um sistema WEB também no caso de o usuário preferir um computador ou notebook ao invés de um dispositivo móvel.  </t>
-  </si>
-  <si>
     <t>A decisão de ser um sistema mobile + web se dá devido à preocupação com usabilidade e fácil integração entre os dois sistemas de controle.</t>
   </si>
   <si>
@@ -479,9 +473,6 @@
   </si>
   <si>
     <t>(---)</t>
-  </si>
-  <si>
-    <t>RF - O sistema deve armazenar as imagens das câmeras na núvem</t>
   </si>
   <si>
     <t>Essa sugestão foi pensanda visando reduzir o custo de ter um HD, SSD ou HD externo de alta capacidade de memória para salvar as imagens das câmeras, sendo necessário apenas HD externo de baixa capacidade de memória para quando a energia cair. Desse modo,  seria possível reduzir o custo do módulo de câmera de segurança e garantir maior disponibilidade e fácil integração das imagens com o sistema de controle de imagens. Um serviço de núvem tal como AWS poderia ser utilizado.</t>
@@ -510,12 +501,120 @@
   <si>
     <t>Pensando em lucros e alcance do produto</t>
   </si>
+  <si>
+    <t>RF - O módulo de câmera de segurança deve possuir uma bateria de duração mínima de 2 horas para oferecer autonomia em caso de falta de energia para que continue a realizar filmagens; RF - O módulo de câmera de segurança deve possuir um led vermelho que deverá acender quando a bateria do módulo estiver prestes a acabar, indicando que o deligará em breve devido a falta de energia; RF - O módulo de fechadura com tranca eletrônica deve possuir chave e tranca convencionais para que também possa funcionar manualmente na falta de energia;   RF - Todos os módulos devem possuir um buzzer e um capacitor para que na falta de energia consigam realizar um alerta sonoro antes do desligamento.</t>
+  </si>
+  <si>
+    <t>As soluções mantêm a segurança, evitam transtornos dos usuários e estavam presentes nas sugestões dos membros, sendo adaptadas conforme discutido na reunião.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF - O módulo de câmera deve possuir um HD externo para armazenar localmente as filmagens na falta de internet; RF - O módulo de câmera de segurança deve enviar as filmagens locais para a núvem quando a internet for reestabelecida e deve limpar o HD externo ao fim da sincronização; RF - Os dispositivos de iluminação devem possuir interruptores convencionais para que seja possível ligar e desligar a iluminação sem dependencia de internet; RF - Os dispositivos de temperatura devem possuir interruptores e interface com botões para que seja possível ligar, desligar, calibrar e interagir sem dependencia de internet;  RF - Os sistemas para controle dos módulos devem emitir um aviso visual por meio da interface alertando aos usuários a falta de internet; RF -  Os módulos de iluminação e termostato devem possuir configuração de horário para que os módulos funcionam de forma autônoma. </t>
+  </si>
+  <si>
+    <t>RF -  Os módulos devem possuir redes isoladas, dificultando o acesso de hackers; Contratar a empresa de Cibersegurança Tempest para utilizarmos suas ferramentas em prol da Cibersegurança dos módulos e do software de controle dos módulos, poupando tempo de desenvolvimento e garantindo qualidade na Cibersegurança.</t>
+  </si>
+  <si>
+    <t>As soluções mantêm a segurança, e visam poupar tempo de desenvolvimento e estavam presentes nas sugestões dos membros, sendo adaptadas conforme discutido na reunião.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF - Deverá ser implementado um sistema mobile para controle dos módulos, visando facilitar o uso dos usuários e um sistema WEB no caso de o usuário preferir um computador ou notebook ao invés de um dispositivo móvel.  </t>
+  </si>
+  <si>
+    <t>A decisão de ser um sistema mobile + web se dá devido à preocupação com usabilidade e fácil integração entre os dois sistemas de controle. Além disso, a decisão tomada foi sugerida por todos os integrantes da equipe.</t>
+  </si>
+  <si>
+    <t>A decisão foi tomada visando reaproveitamento de código, escalabilidade, experiência da equipe com a linguagem JavaScript e os frameworks mencionados e visando poupar tempo no desenvolvimento dos sistemas para controle dos módulos para dedicar mais tempo ao desenvolvimento dos módulos.</t>
+  </si>
+  <si>
+    <t>A arquitetura adoratada deve ser featured-based, uma arquitetura limpa utilizada em projetos React visando escalabilidade</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada porque torna o projeto mais organizado, permite escalabilidade e facilita manutenibilidade.</t>
+  </si>
+  <si>
+    <t>RF - O sistema deve solicitar permissão do usuário para coletar dados referentes aos seus hábitos; RF - O sistema deve, com permissão concedida, coletar informações do usuário tais como: horários comuns em que acende e apaga as luzes, horários de travamento e destravamento das fechaduras, temperaturas preferidas e outros dados referentes aos hábitos de consumo do usuário; RF - O sistema deve utilizar as informações dos hábitos do usuário para gerar inteligência artificial tornando o sistema inteligente e automatizado.</t>
+  </si>
+  <si>
+    <t>As decisões tomadas levaram em conta principalmente a usabilidade.</t>
+  </si>
+  <si>
+    <t>RNF - O sistema deve armazenar as imagens das câmeras na núvem</t>
+  </si>
+  <si>
+    <t>Em um hard-drive no local, ou um solid-state-drive, ou um hard-drive/solid-state-drive externo, para prevenir os casos de falta de energia e internet, e na nuvem utilizando o AWS Cloud Storage</t>
+  </si>
+  <si>
+    <t>RF - O sistema deve armazenar as imagens dos módulos de câmera de segurança na núvem; RNF - O serviço de cloud utilizado para armazenar as imagens dos módulos de câmera de segurança deve ser AWS Cloud Storage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A escolha de armazenar as imagens na núvem é motivado pela redução do custo dos módulos de câmera de segurança visto que esses não necessitarão de um HD ou SSD de alta capacidade de memória, reduzindo o preço dos módulos em questão. A escolha do AWS Cloud Storage deve-se ao fato desse serviço estar disponível em vários países, permitindo maior escalabilidade e sendo útil para outras funcionalidades de cloud. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF - O servidor dos módulos e dos sistemas de controle dos módulos deve ser desenvolvido utilizando linguagem JavaScript e framework NodeJs e quaisquer outros frameworks que forem necessários durante o desenvolvimento. </t>
+  </si>
+  <si>
+    <t>Essa decisão foi sugerida tendo em mente as tecnologias de desenvolvimento front-end sugeridas nas preocupações anteriores, a experiência da equipe de desenvolvimento e a facilidade de desenvolver o servidor e integrá-lo com as demais partes do projeto. Além de que coincide com as sugestões de toda a equipe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para hospedagem do servidor será utilizado o serviço AWS Cloud Hosting Server </t>
+  </si>
+  <si>
+    <t>Pelo suporte oferecido, escalabilidade. Além de que todos os membros da equipe pensaram nessa solução.</t>
+  </si>
+  <si>
+    <t>Os dados do sistema serão armazenados em bancos de dados SQL e NoSQL combinados levando em consideração as diversas finalidades do sistema. O banco de dados SQL utilizado será o PostegreSQL por garantir robustez e o banco de dados DynamoDB do AWS. Ambos os bancos de dados serão alocados nos serviços de cloud da AWS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visto que os sistemas e módulos deverão possuir dados estruturados e desestruturados, uma solução adequada é utilizar bancos de dados SQL e NoSQL juntos para os diversos fins. O banco SQL PostgreSQL  garante robustez e estruturamento dos dados, enquanto o banco NoSQL garante flexibilidade e desempenho em dados desestruturados. O serviço AWS foi escolhido tendo em base que pretendemos utilizá-lo para outros contextos previamente justificados e além disso garante maior disponibilidade e confiabilidade. </t>
+  </si>
+  <si>
+    <t>RNF - Os sistemas para controle dos módulos devem ter idioma inglês para garantir que o sistema seja universal e possa ser vendido em qualquer país; Visto futuramente grande volume de uso por determinada região/país implementaríamos outros idiomas.</t>
+  </si>
+  <si>
+    <t>O idioma inglês foi escolhido tendo em vista maior alcance da aplicação, que a empresa contratante é internacional e  visando tornar a aplicação universal já num primeiro momento, expandindo as regiões de venda e tendo maior lucro.</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada tendo em vista a padronização do código e tendo em vista que a empresa contratante é internacional.</t>
+  </si>
+  <si>
+    <t>RNF - O sistema deve ser codificado em inglês, ou seja, variáveis, funções, classes, parâmetros e etc. devem ser escritos em inglês.</t>
+  </si>
+  <si>
+    <t>RNF - Nomes de variáveis, funções, classes, parâmetros e etc. não devem ser abreviados.</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada visando manutenibilidade do código.</t>
+  </si>
+  <si>
+    <t>RNF - O sistema deve responder às requisições de usuário em no máximo 1 segundo.</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada visando entregar um sistema com melhor desempenho ao usuário.</t>
+  </si>
+  <si>
+    <t>D-001</t>
+  </si>
+  <si>
+    <t>D-002</t>
+  </si>
+  <si>
+    <t>O microcontrolador utilizado para controlar os módulos será o ESP-32.</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada pois o ESP-32 é robusto o suficiente para atender as necessidades dos módulos, além de ser mais barato.</t>
+  </si>
+  <si>
+    <t>A linguagem de programação utilizada para programação dos módulos será C++</t>
+  </si>
+  <si>
+    <t>Essa decisão foi tomada porque a linguagem oficial do microcontrolador ESP-32 é o C++.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -549,6 +648,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -624,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -676,6 +779,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +1015,8 @@
   </sheetPr>
   <dimension ref="A1:D1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2772,7 +2890,9 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2786,13 +2906,13 @@
       <c r="A1" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2847,10 +2967,10 @@
       <c r="D3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -2895,7 +3015,9 @@
       <c r="H4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -2915,15 +3037,33 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -2943,15 +3083,33 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="6"/>
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -2971,15 +3129,33 @@
       <c r="Z6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="6"/>
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -2999,15 +3175,33 @@
       <c r="Z7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="6"/>
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -3027,15 +3221,33 @@
       <c r="Z8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="6"/>
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -3055,15 +3267,33 @@
       <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -3083,15 +3313,33 @@
       <c r="Z10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -3111,15 +3359,33 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -3139,15 +3405,33 @@
       <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -3167,15 +3451,33 @@
       <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="6"/>
+      <c r="A14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -3195,15 +3497,33 @@
       <c r="Z14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="6"/>
+      <c r="A15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -3223,15 +3543,33 @@
       <c r="Z15" s="6"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="A16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -3251,15 +3589,33 @@
       <c r="Z16" s="6"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="A17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -3279,15 +3635,33 @@
       <c r="Z17" s="6"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -3307,15 +3681,33 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="A19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -3335,15 +3727,33 @@
       <c r="Z19" s="6"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="A20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -3363,15 +3773,33 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="A21" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -9747,6 +10175,7 @@
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="D3:H3"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -9760,7 +10189,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10172,10 +10601,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -10208,10 +10637,10 @@
         <v>34</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
@@ -10246,10 +10675,10 @@
         <v>38</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -10282,10 +10711,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
@@ -10322,10 +10751,10 @@
         <v>46</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
@@ -37982,8 +38411,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -37996,7 +38425,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -38108,7 +38537,7 @@
         <v>71</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -38133,10 +38562,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>81</v>
@@ -38148,13 +38577,13 @@
         <v>93</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>81</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -38179,10 +38608,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>81</v>
@@ -38194,13 +38623,13 @@
         <v>93</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -38225,13 +38654,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="D7" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>76</v>
@@ -38240,10 +38669,10 @@
         <v>93</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>81</v>
@@ -38271,10 +38700,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>81</v>
@@ -38289,7 +38718,7 @@
         <v>93</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>76</v>
@@ -38317,13 +38746,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>81</v>
@@ -38335,7 +38764,7 @@
         <v>93</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>76</v>
@@ -38363,13 +38792,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>77</v>
@@ -38381,10 +38810,10 @@
         <v>93</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -38409,13 +38838,13 @@
         <v>27</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>92</v>
@@ -38424,13 +38853,13 @@
         <v>92</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -38455,10 +38884,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>81</v>
@@ -38501,10 +38930,10 @@
         <v>34</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>81</v>
@@ -38519,7 +38948,7 @@
         <v>93</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>77</v>
@@ -38547,16 +38976,16 @@
         <v>38</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>92</v>
@@ -38565,10 +38994,10 @@
         <v>92</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -38593,10 +39022,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>76</v>
@@ -38611,7 +39040,7 @@
         <v>93</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>77</v>
@@ -38639,22 +39068,22 @@
         <v>46</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>77</v>
@@ -45186,7 +45615,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -45199,7 +45628,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -45334,25 +45763,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>109</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -45377,26 +45806,26 @@
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>111</v>
+      <c r="D6" s="15" t="s">
+        <v>107</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>109</v>
-      </c>
       <c r="F6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -45422,25 +45851,25 @@
         <v>12</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>113</v>
-      </c>
       <c r="D7" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -45466,25 +45895,25 @@
         <v>16</v>
       </c>
       <c r="B8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>115</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -45509,26 +45938,26 @@
       <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>117</v>
-      </c>
       <c r="D9" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="H9" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -45554,25 +45983,25 @@
         <v>24</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>119</v>
-      </c>
       <c r="D10" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="H10" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -45598,25 +46027,25 @@
         <v>27</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>121</v>
-      </c>
       <c r="D11" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -45642,25 +46071,25 @@
         <v>31</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>123</v>
+      <c r="D12" s="15" t="s">
+        <v>107</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>109</v>
-      </c>
       <c r="F12" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -45686,10 +46115,10 @@
         <v>34</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -45720,25 +46149,25 @@
         <v>38</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>127</v>
+      <c r="D14" s="15" t="s">
+        <v>107</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>109</v>
-      </c>
       <c r="F14" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -45764,25 +46193,25 @@
         <v>42</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>129</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -45808,25 +46237,25 @@
         <v>46</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>131</v>
-      </c>
       <c r="D16" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>

</xml_diff>